<commit_message>
:sparkles:| All project + include
</commit_message>
<xml_diff>
--- a/Data/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
+++ b/Data/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harghel\Documents\Moi\BTS SIO\bts-portfolio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\Portfolio\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DC5E28-53D3-4C5C-8C72-7B81DE6ECC80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{04AEA206-E523-4AFC-9A65-63D7BEA92C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -147,9 +147,6 @@
     <t>dessin assisté par ordinateur (AutoCAD)</t>
   </si>
   <si>
-    <t>Apprentissage de docker</t>
-  </si>
-  <si>
     <t>28/08/2023 - ….</t>
   </si>
   <si>
@@ -162,24 +159,12 @@
     <t>01/01/2023 - 31/06/2023</t>
   </si>
   <si>
-    <t xml:space="preserve">... - </t>
-  </si>
-  <si>
-    <t xml:space="preserve">… - </t>
-  </si>
-  <si>
     <t>20/12/2023 - 14/06/2023</t>
   </si>
   <si>
     <t>Adresse URL du portfolio : https://portfolioserge7.wordpress.com/#</t>
   </si>
   <si>
-    <t>Intégration d'une BDD en php</t>
-  </si>
-  <si>
-    <t>Création d'une base de donnée workbench</t>
-  </si>
-  <si>
     <t>2022- 2023 45 Heures</t>
   </si>
   <si>
@@ -193,6 +178,33 @@
   </si>
   <si>
     <t>2023 - 2024 ~50H</t>
+  </si>
+  <si>
+    <t>Maintenance d'un projet web interne à l'entreprise</t>
+  </si>
+  <si>
+    <t>04/03/2024 - 31/08/2024</t>
+  </si>
+  <si>
+    <t>… - 04/03/2024</t>
+  </si>
+  <si>
+    <t>... -  04/03/2024</t>
+  </si>
+  <si>
+    <t>Les fondammentaux de Docker</t>
+  </si>
+  <si>
+    <t>Gestion d'une BDD en PHP</t>
+  </si>
+  <si>
+    <t>Schématisation d'une BDD avec MySQL Workbench</t>
+  </si>
+  <si>
+    <t>Mise à jour de fichiers Excel + création de macros en VBA</t>
+  </si>
+  <si>
+    <t>DAO avec AutoCAD</t>
   </si>
 </sst>
 </file>
@@ -1106,13 +1118,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AQ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1187,7 +1199,7 @@
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
@@ -1329,10 +1341,10 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>25</v>
@@ -1341,13 +1353,9 @@
       <c r="E9" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="F9" s="22"/>
       <c r="G9" s="22"/>
-      <c r="H9" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="H9" s="22"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1386,10 +1394,10 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>25</v>
@@ -1397,12 +1405,8 @@
       <c r="D10" s="22"/>
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
-      <c r="G10" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="23"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1441,7 +1445,7 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B11" s="8">
         <v>2023</v>
@@ -1455,9 +1459,7 @@
       <c r="G11" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="H11" s="23"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1496,10 +1498,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>25</v>
@@ -1508,9 +1510,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="22"/>
-      <c r="F12" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="F12" s="22"/>
       <c r="G12" s="22"/>
       <c r="H12" s="23"/>
       <c r="I12"/>
@@ -1551,23 +1551,17 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>25</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
       <c r="E13" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="F13" s="22"/>
       <c r="G13" s="22" t="s">
         <v>25</v>
       </c>
@@ -1707,7 +1701,7 @@
         <v>27</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>25</v>
@@ -1718,9 +1712,7 @@
       <c r="E16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="F16" s="22"/>
       <c r="G16" s="22" t="s">
         <v>25</v>
       </c>
@@ -1763,25 +1755,19 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="22" t="s">
         <v>25</v>
       </c>
       <c r="E17" s="22"/>
-      <c r="F17" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1823,7 +1809,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="22"/>
       <c r="D18" s="22" t="s">
@@ -1838,9 +1824,7 @@
       <c r="G18" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H18" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="H18" s="23"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1926,25 +1910,19 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C20" s="22"/>
       <c r="D20" s="22" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="22"/>
-      <c r="F20" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H20" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="23"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1983,10 +1961,10 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22" t="s">
@@ -2001,9 +1979,7 @@
       <c r="G21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="23" t="s">
-        <v>25</v>
-      </c>
+      <c r="H21" s="23"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -2041,14 +2017,24 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="8"/>
+      <c r="A22" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="15"/>
+      <c r="D22" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="23"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>

</xml_diff>

<commit_message>
:sparkles:| creating the file repertoire.php and fixing some other files
</commit_message>
<xml_diff>
--- a/Data/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
+++ b/Data/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\Portfolio\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{04AEA206-E523-4AFC-9A65-63D7BEA92C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CC97AA-C977-426D-A899-CC76E527213D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24" yWindow="24" windowWidth="23016" windowHeight="12216" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$27</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$31</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -162,9 +162,6 @@
     <t>20/12/2023 - 14/06/2023</t>
   </si>
   <si>
-    <t>Adresse URL du portfolio : https://portfolioserge7.wordpress.com/#</t>
-  </si>
-  <si>
     <t>2022- 2023 45 Heures</t>
   </si>
   <si>
@@ -205,6 +202,33 @@
   </si>
   <si>
     <t>DAO avec AutoCAD</t>
+  </si>
+  <si>
+    <t>Adresse URL du portfolio : https://sergeharghel.fr</t>
+  </si>
+  <si>
+    <t>Projet 1 Création d'un logiciel de gestion d'un magasin</t>
+  </si>
+  <si>
+    <t>Projet 2 Création d'un site de veille Laravel</t>
+  </si>
+  <si>
+    <t>Projet 3 Création d'une application Place de théatre</t>
+  </si>
+  <si>
+    <t>Projet 4 Création d'un simulateur immobilier avec Electron</t>
+  </si>
+  <si>
+    <t>01/08/2023 au 01/01/2024</t>
+  </si>
+  <si>
+    <t>29/01/2024 au 02/02/2024</t>
+  </si>
+  <si>
+    <t>12/02/2024 au 02/03/2024</t>
+  </si>
+  <si>
+    <t>11/03/2024 au 30/04/2024</t>
   </si>
 </sst>
 </file>
@@ -1121,10 +1145,10 @@
   <sheetPr codeName="Sheet1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AQ73"/>
+  <dimension ref="A1:AQ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1223,7 @@
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="35" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="B5" s="36"/>
       <c r="C5" s="36"/>
@@ -1341,7 +1365,7 @@
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="21" t="s">
         <v>33</v>
@@ -1394,10 +1418,10 @@
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>25</v>
@@ -1445,7 +1469,7 @@
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="8">
         <v>2023</v>
@@ -1498,10 +1522,10 @@
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>25</v>
@@ -1551,10 +1575,10 @@
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="22"/>
       <c r="D13" s="22"/>
@@ -1605,14 +1629,26 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="22"/>
+      <c r="A14" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="23"/>
+      <c r="F14" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1649,17 +1685,27 @@
       <c r="AP14"/>
       <c r="AQ14"/>
     </row>
-    <row r="15" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="31"/>
-      <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
+    <row r="15" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1698,25 +1744,25 @@
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="G16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H16" s="23"/>
+      <c r="H16" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1755,19 +1801,25 @@
     </row>
     <row r="17" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22" t="s">
-        <v>25</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="22"/>
       <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="23"/>
+      <c r="F17" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" s="23" t="s">
+        <v>25</v>
+      </c>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1805,25 +1857,13 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="A18" s="9"/>
+      <c r="B18" s="8"/>
       <c r="C18" s="22"/>
-      <c r="D18" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
       <c r="H18" s="23"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -1863,7 +1903,7 @@
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
@@ -1910,18 +1950,24 @@
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="22"/>
+        <v>32</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="D20" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="22"/>
+      <c r="E20" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
+      <c r="G20" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="H20" s="23"/>
       <c r="I20"/>
       <c r="J20"/>
@@ -1961,24 +2007,18 @@
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C21" s="22"/>
       <c r="D21" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="G21" s="22" t="s">
-        <v>25</v>
-      </c>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="22"/>
       <c r="H21" s="23"/>
       <c r="I21"/>
       <c r="J21"/>
@@ -2018,16 +2058,18 @@
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="14"/>
+        <v>29</v>
+      </c>
+      <c r="C22" s="22"/>
       <c r="D22" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="22"/>
+      <c r="E22" s="22" t="s">
+        <v>25</v>
+      </c>
       <c r="F22" s="22" t="s">
         <v>25</v>
       </c>
@@ -2071,15 +2113,17 @@
       <c r="AP22"/>
       <c r="AQ22"/>
     </row>
-    <row r="23" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="15"/>
+    <row r="23" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
+      <c r="A23" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="32"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2117,14 +2161,20 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="15"/>
+      <c r="A24" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="23"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2162,14 +2212,26 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="15"/>
+      <c r="A25" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="23"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2206,15 +2268,25 @@
       <c r="AP25"/>
       <c r="AQ25"/>
     </row>
-    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="10"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="17"/>
+    <row r="26" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="23"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2251,15 +2323,15 @@
       <c r="AP26"/>
       <c r="AQ26"/>
     </row>
-    <row r="27" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A27" s="5"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
+    <row r="27" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="15"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2296,10 +2368,186 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="15"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+      <c r="Z28"/>
+      <c r="AA28"/>
+      <c r="AB28"/>
+      <c r="AC28"/>
+      <c r="AD28"/>
+      <c r="AE28"/>
+      <c r="AF28"/>
+      <c r="AG28"/>
+      <c r="AH28"/>
+      <c r="AI28"/>
+      <c r="AJ28"/>
+      <c r="AK28"/>
+      <c r="AL28"/>
+      <c r="AM28"/>
+      <c r="AN28"/>
+      <c r="AO28"/>
+      <c r="AP28"/>
+      <c r="AQ28"/>
+    </row>
+    <row r="29" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="15"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+      <c r="Z29"/>
+      <c r="AA29"/>
+      <c r="AB29"/>
+      <c r="AC29"/>
+      <c r="AD29"/>
+      <c r="AE29"/>
+      <c r="AF29"/>
+      <c r="AG29"/>
+      <c r="AH29"/>
+      <c r="AI29"/>
+      <c r="AJ29"/>
+      <c r="AK29"/>
+      <c r="AL29"/>
+      <c r="AM29"/>
+      <c r="AN29"/>
+      <c r="AO29"/>
+      <c r="AP29"/>
+      <c r="AQ29"/>
+    </row>
+    <row r="30" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="17"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+      <c r="Z30"/>
+      <c r="AA30"/>
+      <c r="AB30"/>
+      <c r="AC30"/>
+      <c r="AD30"/>
+      <c r="AE30"/>
+      <c r="AF30"/>
+      <c r="AG30"/>
+      <c r="AH30"/>
+      <c r="AI30"/>
+      <c r="AJ30"/>
+      <c r="AK30"/>
+      <c r="AL30"/>
+      <c r="AM30"/>
+      <c r="AN30"/>
+      <c r="AO30"/>
+      <c r="AP30"/>
+      <c r="AQ30"/>
+    </row>
+    <row r="31" spans="1:43" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+      <c r="Z31"/>
+      <c r="AA31"/>
+      <c r="AB31"/>
+      <c r="AC31"/>
+      <c r="AD31"/>
+      <c r="AE31"/>
+      <c r="AF31"/>
+      <c r="AG31"/>
+      <c r="AH31"/>
+      <c r="AI31"/>
+      <c r="AJ31"/>
+      <c r="AK31"/>
+      <c r="AL31"/>
+      <c r="AM31"/>
+      <c r="AN31"/>
+      <c r="AO31"/>
+      <c r="AP31"/>
+      <c r="AQ31"/>
+    </row>
     <row r="32" spans="1:43" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="33" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2342,6 +2590,10 @@
     <row r="71" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="72" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="73" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
     <mergeCell ref="G1:H1"/>
@@ -2352,8 +2604,8 @@
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A15:H15"/>
     <mergeCell ref="A19:H19"/>
+    <mergeCell ref="A23:H23"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
   </mergeCells>

</xml_diff>

<commit_message>
:sparkles:| addding legals.php and work10
</commit_message>
<xml_diff>
--- a/Data/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
+++ b/Data/6- Annexe 6-1 - Tableau de synthèse - Epreuve E4 - BTS SIO 2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MAMP\htdocs\Portfolio\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C13387-D925-4AA9-AA62-92F52F5AAD76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401F0319-8F6D-4B6C-8B5A-06EA3886301E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="59">
   <si>
     <t>BTS SERVICES INFORMATIQUES AUX ORGANISATIONS</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>SESSION 2024</t>
+  </si>
+  <si>
+    <t>Création d'un script Bash</t>
+  </si>
+  <si>
+    <t>01/01/2024 au 05/01/2024</t>
   </si>
 </sst>
 </file>
@@ -771,9 +777,48 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -796,45 +841,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1147,8 +1153,8 @@
   </sheetPr>
   <dimension ref="A1:AQ77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1161,56 +1167,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="24"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:43" ht="41.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="31" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="26"/>
-      <c r="H3" s="32"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="45"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="30"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="12" t="s">
         <v>3</v>
       </c>
@@ -1222,22 +1228,22 @@
       </c>
     </row>
     <row r="5" spans="1:43" ht="39.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="43" t="s">
+      <c r="A5" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="44"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="44"/>
-      <c r="H5" s="45"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="37"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="33" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1260,8 +1266,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="324.89999999999998" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="34"/>
-      <c r="B7" s="42"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="19" t="s">
         <v>13</v>
       </c>
@@ -1317,16 +1323,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="37"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="29"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1857,13 +1863,19 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="39.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>58</v>
+      </c>
       <c r="C18" s="22"/>
       <c r="D18" s="22"/>
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
+      <c r="G18" s="22" t="s">
+        <v>23</v>
+      </c>
       <c r="H18" s="23"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -1902,16 +1914,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="40"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="32"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2114,16 +2126,16 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="40"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="32"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2596,6 +2608,11 @@
     <row r="77" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2603,11 +2620,6 @@
     <mergeCell ref="A23:H23"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2618,6 +2630,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010047EF1D24E1AA4E498929CCAFDB10CE83" ma:contentTypeVersion="3" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="dd875bf50724420782c9497fbe3f1275">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="db57f7ab-da79-497d-a478-0254fd781a28" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="941c9eaedf1073e70d2cd50b7bcbdb6b" ns2:_="">
     <xsd:import namespace="db57f7ab-da79-497d-a478-0254fd781a28"/>
@@ -2755,15 +2776,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2771,6 +2783,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B910F78D-3099-4E05-86CC-AFF909CA5375}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DE0AE58F-B387-41A0-9F53-279B2DE065FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2788,14 +2808,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B910F78D-3099-4E05-86CC-AFF909CA5375}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92BEB1BE-8A88-467B-80B7-8FACF9956796}">
   <ds:schemaRefs>

</xml_diff>